<commit_message>
predicted retention time for SRM peptide
</commit_message>
<xml_diff>
--- a/analyses/DNR_TransitionSelection_20170707/2017-07-08-Final-Transitions/2017-07-11-Predicted-SRM-Retention-Times.xlsx
+++ b/analyses/DNR_TransitionSelection_20170707/2017-07-08-Final-Transitions/2017-07-11-Predicted-SRM-Retention-Times.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="76">
   <si>
     <t>PRTC</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>Average SRM Retention Time</t>
+  </si>
+  <si>
+    <t>TASEEFDSAIAQDK</t>
   </si>
 </sst>
 </file>
@@ -523,11 +526,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="102235312"/>
-        <c:axId val="103045072"/>
+        <c:axId val="869039792"/>
+        <c:axId val="890599280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102235312"/>
+        <c:axId val="869039792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80.0"/>
@@ -633,12 +636,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103045072"/>
+        <c:crossAx val="890599280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103045072"/>
+        <c:axId val="890599280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35.0"/>
@@ -739,7 +742,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="102235312"/>
+        <c:crossAx val="869039792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1645,7 +1648,7 @@
   <dimension ref="A1:N901"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1897,6 +1900,16 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8">
+        <v>48</v>
+      </c>
+      <c r="C8">
+        <f>(0.2758*48) + 11.409</f>
+        <v>24.647399999999998</v>
+      </c>
       <c r="H8" t="s">
         <v>10</v>
       </c>

</xml_diff>